<commit_message>
Added cloud effect, flip effect, and 3d slider practice. Edit my dream car and bouncing ball practice
</commit_message>
<xml_diff>
--- a/Cross-Broswer-Summary.xlsx
+++ b/Cross-Broswer-Summary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
   <si>
     <t>IE6</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -64,12 +64,16 @@
     <t>Supprot</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Border-radius</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,6 +117,24 @@
       <sz val="16"/>
       <color rgb="FF008000"/>
       <name val="Arial Rounded MT Bold"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -184,8 +206,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -212,8 +240,14 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -545,7 +579,7 @@
   <dimension ref="A1:I181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -859,16 +893,34 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="1"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+    <row r="25" spans="1:9" ht="19">
+      <c r="A25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="8"/>
@@ -1341,6 +1393,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>